<commit_message>
GSCHED-844: Fix OCS telescope calendar with wrong Programs
</commit_message>
<xml_diff>
--- a/scheduler/services/resource/data/validation/telescope_schedules.xlsx
+++ b/scheduler/services/resource/data/validation/telescope_schedules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergio.troncoso/PycharmProjects/scheduler/scheduler/services/resource/data/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9E245E-8B56-0644-8B02-05E621FC0D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F720B46-9973-CD4F-BD99-9DF54021C440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35900" yWindow="1800" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -275,10 +275,10 @@
     <t>PV: GN-2019A-C-1</t>
   </si>
   <si>
-    <t>Visitor: `Alopeke | Partner: KR</t>
+    <t>Queue | Partner: KR</t>
   </si>
   <si>
-    <t>Queue | Partner: KR</t>
+    <t xml:space="preserve">Queue </t>
   </si>
 </sst>
 </file>
@@ -42635,10 +42635,10 @@
   <dimension ref="A1:W548"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B221" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B254" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C270" sqref="C270"/>
+      <selection pane="bottomRight" activeCell="C285" sqref="C285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -61244,7 +61244,7 @@
         <v>25</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D271" s="1" t="s">
         <v>27</v>
@@ -61382,7 +61382,7 @@
         <v>25</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="D273" s="1" t="s">
         <v>27</v>
@@ -63383,7 +63383,7 @@
         <v>25</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="D302" s="1" t="s">
         <v>27</v>
@@ -63452,7 +63452,7 @@
         <v>25</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="D303" s="1" t="s">
         <v>27</v>
@@ -63521,7 +63521,7 @@
         <v>25</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="D304" s="1" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
GSCHED-844: Fix missing sToOs (#591)
* GSCHED-844: Fix missing sToOs on plans

* GSCHED-844: Fix missing sToOs on plans

* GSCHED-844: Fix OCS telescope calendar with wrong Programs
</commit_message>
<xml_diff>
--- a/scheduler/services/resource/data/validation/telescope_schedules.xlsx
+++ b/scheduler/services/resource/data/validation/telescope_schedules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergio.troncoso/PycharmProjects/scheduler/scheduler/services/resource/data/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9E245E-8B56-0644-8B02-05E621FC0D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F720B46-9973-CD4F-BD99-9DF54021C440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35900" yWindow="1800" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -275,10 +275,10 @@
     <t>PV: GN-2019A-C-1</t>
   </si>
   <si>
-    <t>Visitor: `Alopeke | Partner: KR</t>
+    <t>Queue | Partner: KR</t>
   </si>
   <si>
-    <t>Queue | Partner: KR</t>
+    <t xml:space="preserve">Queue </t>
   </si>
 </sst>
 </file>
@@ -42635,10 +42635,10 @@
   <dimension ref="A1:W548"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B221" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B254" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C270" sqref="C270"/>
+      <selection pane="bottomRight" activeCell="C285" sqref="C285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -61244,7 +61244,7 @@
         <v>25</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D271" s="1" t="s">
         <v>27</v>
@@ -61382,7 +61382,7 @@
         <v>25</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="D273" s="1" t="s">
         <v>27</v>
@@ -63383,7 +63383,7 @@
         <v>25</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="D302" s="1" t="s">
         <v>27</v>
@@ -63452,7 +63452,7 @@
         <v>25</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="D303" s="1" t="s">
         <v>27</v>
@@ -63521,7 +63521,7 @@
         <v>25</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="D304" s="1" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
GSCHED-927: Add missing modes to the calendar
</commit_message>
<xml_diff>
--- a/scheduler/services/resource/data/validation/telescope_schedules.xlsx
+++ b/scheduler/services/resource/data/validation/telescope_schedules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergio.troncoso/PycharmProjects/scheduler/scheduler/services/resource/data/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F720B46-9973-CD4F-BD99-9DF54021C440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB68D29-82FC-4C49-A6F8-A5F2E0F30DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35900" yWindow="1800" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GS" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24007" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24007" uniqueCount="87">
   <si>
     <t>Local Date</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t xml:space="preserve">Queue </t>
+  </si>
+  <si>
+    <t>Queue | Visitor: `Alopeke</t>
   </si>
 </sst>
 </file>
@@ -42635,10 +42638,10 @@
   <dimension ref="A1:W548"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B254" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B170" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C285" sqref="C285"/>
+      <selection pane="bottomRight" activeCell="R211" sqref="R211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -56044,7 +56047,7 @@
         <v>25</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>27</v>
@@ -57148,7 +57151,7 @@
         <v>25</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>33</v>
@@ -57188,7 +57191,7 @@
         <v>30</v>
       </c>
       <c r="Q211" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R211" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
GSCHED-927: Add missing modes to the calendar (#665)
</commit_message>
<xml_diff>
--- a/scheduler/services/resource/data/validation/telescope_schedules.xlsx
+++ b/scheduler/services/resource/data/validation/telescope_schedules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergio.troncoso/PycharmProjects/scheduler/scheduler/services/resource/data/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F720B46-9973-CD4F-BD99-9DF54021C440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB68D29-82FC-4C49-A6F8-A5F2E0F30DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35900" yWindow="1800" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GS" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24007" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24007" uniqueCount="87">
   <si>
     <t>Local Date</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t xml:space="preserve">Queue </t>
+  </si>
+  <si>
+    <t>Queue | Visitor: `Alopeke</t>
   </si>
 </sst>
 </file>
@@ -42635,10 +42638,10 @@
   <dimension ref="A1:W548"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B254" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B170" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C285" sqref="C285"/>
+      <selection pane="bottomRight" activeCell="R211" sqref="R211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -56044,7 +56047,7 @@
         <v>25</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>27</v>
@@ -57148,7 +57151,7 @@
         <v>25</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>33</v>
@@ -57188,7 +57191,7 @@
         <v>30</v>
       </c>
       <c r="Q211" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R211" s="1" t="s">
         <v>30</v>

</xml_diff>